<commit_message>
commits as of 26/04/2020
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
+++ b/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18780" windowHeight="3810" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19050" windowHeight="8040" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CreateRecipient" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Number</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Updated First Name</t>
   </si>
   <si>
-    <t>Fax Address Updated</t>
-  </si>
-  <si>
     <t>Modify Reason</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Fax Number</t>
   </si>
   <si>
-    <t>Fax Address Recipient&lt;9987288&gt;</t>
-  </si>
-  <si>
     <t>Recipient1</t>
   </si>
   <si>
@@ -92,16 +86,25 @@
     <t>Name1</t>
   </si>
   <si>
-    <t>Fax Address Recipient&lt;9987288&gt;,SampleData&lt;123467&gt;</t>
-  </si>
-  <si>
     <t>Fax Address Updated Recipient&lt;9987288&gt;,SampleData&lt;123467&gt;</t>
   </si>
   <si>
     <t>sample2 delete&lt;12345&gt;</t>
   </si>
   <si>
-    <t>Fax Address Recipient&lt;9987288&gt;,sample2 delete&lt;12345&gt;</t>
+    <t>TrialData</t>
+  </si>
+  <si>
+    <t>Recepient Updated</t>
+  </si>
+  <si>
+    <t>TrialData Recipient&lt;9987288&gt;</t>
+  </si>
+  <si>
+    <t>TrialData Recipient&lt;9987288&gt;,sample2 delete&lt;12345&gt;</t>
+  </si>
+  <si>
+    <t>radsooo</t>
   </si>
 </sst>
 </file>
@@ -453,28 +456,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -493,7 +499,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,24 +511,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -531,10 +537,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -544,10 +550,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,21 +564,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -581,7 +587,12 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -593,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,19 +618,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,13 +638,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>25</v>
@@ -650,7 +661,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,22 +676,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -688,19 +699,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -713,41 +724,41 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E21" sqref="E21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="3" max="3" width="60.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commits as of 27/4/2020
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
+++ b/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>Number</t>
   </si>
@@ -104,7 +104,13 @@
     <t>TrialData Recipient&lt;9987288&gt;,sample2 delete&lt;12345&gt;</t>
   </si>
   <si>
-    <t>radsooo</t>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>500000</t>
   </si>
 </sst>
 </file>
@@ -457,7 +463,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +511,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -553,7 +560,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +600,15 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit as of 4th may2020
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
+++ b/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\scripts\ocms\src\test\resources\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19050" windowHeight="8040" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22890" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="CreateRecipient" sheetId="1" r:id="rId1"/>
@@ -20,11 +15,12 @@
     <sheet name="DeleteAddressBook" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:U24"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>Number</t>
   </si>
@@ -35,9 +31,6 @@
     <t>Recipient</t>
   </si>
   <si>
-    <t>9987288</t>
-  </si>
-  <si>
     <t>Updated First Name</t>
   </si>
   <si>
@@ -59,9 +52,6 @@
     <t>FaxLine</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
     <t>Fax Number</t>
   </si>
   <si>
@@ -86,24 +76,12 @@
     <t>Name1</t>
   </si>
   <si>
-    <t>Fax Address Updated Recipient&lt;9987288&gt;,SampleData&lt;123467&gt;</t>
-  </si>
-  <si>
-    <t>sample2 delete&lt;12345&gt;</t>
-  </si>
-  <si>
     <t>TrialData</t>
   </si>
   <si>
     <t>Recepient Updated</t>
   </si>
   <si>
-    <t>TrialData Recipient&lt;9987288&gt;</t>
-  </si>
-  <si>
-    <t>TrialData Recipient&lt;9987288&gt;,sample2 delete&lt;12345&gt;</t>
-  </si>
-  <si>
     <t>radsooo</t>
   </si>
   <si>
@@ -120,6 +98,33 @@
   </si>
   <si>
     <t>deleted</t>
+  </si>
+  <si>
+    <t>Palak Garg&lt;9917186286&gt;</t>
+  </si>
+  <si>
+    <t>10384</t>
+  </si>
+  <si>
+    <t>91827</t>
+  </si>
+  <si>
+    <t>TrialData Recipient&lt;91827&gt;</t>
+  </si>
+  <si>
+    <t>TrialData Recipient&lt;991827&gt;,Palak Garg&lt;9917186286&gt;</t>
+  </si>
+  <si>
+    <t>TrialData Recipient&lt;91827&gt;,Palak Garg&lt;9917186286&gt;</t>
+  </si>
+  <si>
+    <t>Recepient Updated Recipient&lt;91827&gt;,Palak Garg&lt;9917186286&gt;</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>918279</t>
   </si>
 </sst>
 </file>
@@ -476,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,24 +496,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -521,12 +534,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
@@ -534,36 +548,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -573,72 +587,84 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="C1:D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>982332</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -652,32 +678,32 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -685,16 +711,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -708,7 +734,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,22 +749,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -746,19 +772,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -771,7 +797,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:E22"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,30 +808,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit as of 4th may 2020
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
+++ b/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22890" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17415" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="CreateRecipient" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>Number</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>918279</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>27</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,6 +528,28 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commits as of 5th may 2020
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
+++ b/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17415" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16785" windowHeight="5145"/>
   </bookViews>
   <sheets>
     <sheet name="CreateRecipient" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="DeleteAddressBook" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:U24"/>
+  <oleSize ref="A1:N15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>Number</t>
   </si>
@@ -131,6 +131,18 @@
   </si>
   <si>
     <t>27</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -490,7 +502,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +574,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +611,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -618,7 +630,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +662,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -703,10 +715,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>29</v>
@@ -748,6 +760,40 @@
         <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commits as of 6thmay2020
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
+++ b/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16785" windowHeight="5145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="8040" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="CreateRecipient" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,16 @@
     <sheet name="AddressCreate" sheetId="4" r:id="rId4"/>
     <sheet name="EditAddressBook" sheetId="5" r:id="rId5"/>
     <sheet name="DeleteAddressBook" sheetId="6" r:id="rId6"/>
+    <sheet name="RecipientQuery" sheetId="12" r:id="rId7"/>
+    <sheet name="AddressBookQuery" sheetId="13" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N15"/>
+  <oleSize ref="A1:O19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
   <si>
     <t>Number</t>
   </si>
@@ -143,6 +145,26 @@
   </si>
   <si>
     <t>1000</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>SELECT 
+    [FirstName] as 'Name1'
+    ,[LastName] as 'Name2'
+    ,[FaxNumber] as 'Fax Number'
+    ,[LastChangedBy] as 'Last Changed By'
+    ,[LastChangedOn] as 'Last Changed On'
+    FROM [Fax_Recipient]</t>
+  </si>
+  <si>
+    <t>SELECT 
+  [Name] as Name
+  ,[FaxLine] as 'Fax Line'
+  ,[LastChangedBy] as 'Last Changed By'
+  ,[LastChangedOn] as 'Last Changed On'
+  FROM [Fax_AddressBook]</t>
   </si>
 </sst>
 </file>
@@ -190,11 +212,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -911,4 +936,60 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commits as of today
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
+++ b/ocms/src/test/resources/TestData/FaxAddressBookData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="8040" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22890" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="CreateRecipient" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="AddressBookQuery" sheetId="13" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O19"/>
+  <oleSize ref="A1:U24"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
   <si>
     <t>Number</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Palak Garg&lt;9917186286&gt;</t>
-  </si>
-  <si>
-    <t>10384</t>
   </si>
   <si>
     <t>91827</t>
@@ -526,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -556,15 +553,15 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,7 +572,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -586,7 +583,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -687,7 +684,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -723,10 +720,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -742,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,33 +773,33 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -810,16 +807,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -833,7 +830,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,16 +868,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -896,7 +893,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,10 +921,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -953,12 +950,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -970,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,12 +978,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>